<commit_message>
Added Semantic Chunking strategies
</commit_message>
<xml_diff>
--- a/datasets/acme_spd/evaluations/llamaindex/data/ACME_SPD_MINI_S003_00_GM_command-r_EM_embed-english-v3.0_P_1024_K_3_2024-05-05.xlsx
+++ b/datasets/acme_spd/evaluations/llamaindex/data/ACME_SPD_MINI_S003_00_GM_command-r_EM_embed-english-v3.0_P_1024_K_3_2024-05-05.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\rag_tester_llidx\datasets\acme_spd\evaluations\llamaindex\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A216DF2-FCE5-4210-8824-68052C50BD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Faithfulness" sheetId="5" r:id="rId5"/>
     <sheet name="Token Counts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -5874,8 +5880,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5938,13 +5944,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5982,7 +5996,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -6016,6 +6030,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -6050,9 +6065,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6225,14 +6241,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6294,7 +6312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -6344,7 +6362,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -6394,7 +6412,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6411,7 +6429,7 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G4" t="s">
         <v>164</v>
@@ -6444,7 +6462,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -6461,7 +6479,7 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>0.8333333333333334</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G5" t="s">
         <v>164</v>
@@ -6494,7 +6512,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -6544,7 +6562,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -6594,7 +6612,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6644,7 +6662,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -6694,7 +6712,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -6711,7 +6729,7 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G10" t="s">
         <v>164</v>
@@ -6744,7 +6762,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -6794,7 +6812,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -6844,7 +6862,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -6861,7 +6879,7 @@
         <v>4</v>
       </c>
       <c r="F13">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G13" t="s">
         <v>164</v>
@@ -6894,7 +6912,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -6944,7 +6962,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -6961,7 +6979,7 @@
         <v>5</v>
       </c>
       <c r="F15">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G15" t="s">
         <v>164</v>
@@ -6994,7 +7012,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -7044,7 +7062,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -7094,7 +7112,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -7144,7 +7162,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -7194,7 +7212,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -7244,7 +7262,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -7294,7 +7312,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -7344,7 +7362,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -7394,7 +7412,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -7444,7 +7462,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -7494,7 +7512,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -7511,7 +7529,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>0.8888888888888888</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="G26" t="s">
         <v>164</v>
@@ -7544,7 +7562,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -7594,7 +7612,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -7644,7 +7662,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -7661,7 +7679,7 @@
         <v>3</v>
       </c>
       <c r="F29">
-        <v>0.9090909090909091</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="G29" t="s">
         <v>164</v>
@@ -7694,7 +7712,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -7744,7 +7762,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -7794,7 +7812,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -7844,7 +7862,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -7894,7 +7912,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -7944,7 +7962,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -7994,7 +8012,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -8044,7 +8062,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -8100,14 +8118,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8127,7 +8147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -8144,7 +8164,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -8161,7 +8181,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -8178,7 +8198,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -8198,7 +8218,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -8218,7 +8238,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -8232,7 +8252,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -8252,7 +8272,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -8266,7 +8286,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -8286,7 +8306,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -8303,7 +8323,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -8320,7 +8340,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -8337,7 +8357,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -8354,7 +8374,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -8371,7 +8391,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -8391,7 +8411,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -8408,7 +8428,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -8425,7 +8445,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -8442,7 +8462,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -8459,7 +8479,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -8476,7 +8496,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -8493,7 +8513,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -8507,7 +8527,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -8524,7 +8544,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -8544,7 +8564,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -8561,7 +8581,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -8575,7 +8595,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -8592,7 +8612,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -8609,7 +8629,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -8623,7 +8643,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -8643,7 +8663,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -8660,7 +8680,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -8674,7 +8694,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -8688,7 +8708,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -8702,7 +8722,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -8716,7 +8736,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -8742,14 +8762,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>243</v>
       </c>
@@ -8760,7 +8780,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -8768,10 +8788,10 @@
         <v>126.5</v>
       </c>
       <c r="C2">
-        <v>30.69678932178932</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>30.696789321789321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>243</v>
       </c>
@@ -8782,15 +8802,15 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>247</v>
       </c>
       <c r="B7">
-        <v>3.513888888888889</v>
+        <v>3.5138888888888888</v>
       </c>
       <c r="C7">
-        <v>0.8526885922719257</v>
+        <v>0.85268859227192573</v>
       </c>
     </row>
   </sheetData>
@@ -8799,14 +8819,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="6" max="6" width="54" customWidth="1"/>
+    <col min="7" max="7" width="43.921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8829,7 +8853,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -8849,7 +8873,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -8869,7 +8893,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -8889,7 +8913,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -8909,7 +8933,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -8929,7 +8953,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -8949,7 +8973,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -8969,7 +8993,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -8989,7 +9013,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -9009,7 +9033,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -9029,7 +9053,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -9049,7 +9073,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -9069,7 +9093,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -9089,7 +9113,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -9109,7 +9133,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -9129,7 +9153,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -9149,7 +9173,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -9169,7 +9193,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -9189,7 +9213,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -9209,7 +9233,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -9229,7 +9253,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -9249,7 +9273,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -9269,7 +9293,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -9289,7 +9313,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -9309,7 +9333,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -9329,7 +9353,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -9349,7 +9373,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -9369,7 +9393,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -9389,7 +9413,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -9409,7 +9433,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -9429,7 +9453,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -9449,7 +9473,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -9469,7 +9493,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -9489,7 +9513,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -9509,7 +9533,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -9529,7 +9553,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -9555,14 +9579,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9585,7 +9609,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -9605,7 +9629,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -9625,7 +9649,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9639,13 +9663,13 @@
         <v>130</v>
       </c>
       <c r="E4">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -9659,13 +9683,13 @@
         <v>131</v>
       </c>
       <c r="E5">
-        <v>0.8333333333333334</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -9685,7 +9709,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -9705,7 +9729,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -9725,7 +9749,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -9745,7 +9769,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -9759,13 +9783,13 @@
         <v>136</v>
       </c>
       <c r="E10">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F10" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -9785,7 +9809,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -9805,7 +9829,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -9819,13 +9843,13 @@
         <v>139</v>
       </c>
       <c r="E13">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F13" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -9845,7 +9869,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -9859,13 +9883,13 @@
         <v>141</v>
       </c>
       <c r="E15">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F15" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -9885,7 +9909,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -9905,7 +9929,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -9925,7 +9949,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -9945,7 +9969,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -9965,7 +9989,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -9985,7 +10009,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -10005,7 +10029,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -10025,7 +10049,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -10045,7 +10069,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -10065,7 +10089,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -10079,13 +10103,13 @@
         <v>152</v>
       </c>
       <c r="E26">
-        <v>0.8888888888888888</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="F26" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -10105,7 +10129,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -10125,7 +10149,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -10139,13 +10163,13 @@
         <v>155</v>
       </c>
       <c r="E29">
-        <v>0.9090909090909091</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="F29" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -10165,7 +10189,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -10185,7 +10209,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -10205,7 +10229,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -10225,7 +10249,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -10245,7 +10269,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -10265,7 +10289,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -10285,7 +10309,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -10311,14 +10335,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>322</v>
       </c>
@@ -10329,7 +10353,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>606898</v>
       </c>

</xml_diff>